<commit_message>
removed tool owners pii
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694EBE6E-7851-4BCC-B8F8-55C4B7B77D1B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DC1524-8554-40EB-A5EF-0DF2566C61DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADS" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Powershell(y/n)</t>
   </si>
   <si>
-    <t>ntuttle</t>
-  </si>
-  <si>
     <t>the purpose of...</t>
   </si>
   <si>
@@ -69,18 +66,12 @@
     <t>PKI_CA script collects data for Certification Server role of ADCS. It is batch script. Please note that it will collect only CA servier side data for this single role and that it is highly recommended to run Authentication data collection script in parallel</t>
   </si>
   <si>
-    <t>milanmil</t>
-  </si>
-  <si>
     <t>PKI_CEP_CES</t>
   </si>
   <si>
     <t>PKI_CEP_CES script collects data for CEP (Certificate Enrollment Policy) and CES (Certificate Enrollment Services) roles (together aka WES/Web Enrollment Services) of ADCS. It is batch script. Please note that it will collect only CEP/CES server side data for those two roles and that it is highly recommended to run Authentication data collection script in parallel.</t>
   </si>
   <si>
-    <t>tolui</t>
-  </si>
-  <si>
     <t>certquery.dll</t>
   </si>
   <si>
@@ -99,9 +90,6 @@
     <t>PKI_Scard script collects Smartcard Subsystem relevant data. It includes components that run as part of the client app that uses smartcard certificate and smartcard resource manager service. It is batch script. Please note that it will collect only cient side data related to Windows smartcard subsystem.</t>
   </si>
   <si>
-    <t>mnicolae</t>
-  </si>
-  <si>
     <t>PKI_Credential_Roaming</t>
   </si>
   <si>
@@ -112,9 +100,6 @@
   </si>
   <si>
     <t>AD_PERF</t>
-  </si>
-  <si>
-    <t>waynmc</t>
   </si>
   <si>
     <t xml:space="preserve">AD Perf Data Collection Tool is powershell script for tracing several scenarios: 
@@ -127,13 +112,7 @@
 7: Long Term Baseline performance of a Domain Controller; </t>
   </si>
   <si>
-    <t>boussom; tolui</t>
-  </si>
-  <si>
     <t>PKI_EFS</t>
-  </si>
-  <si>
-    <t>mnicolae; milanmil</t>
   </si>
   <si>
     <t>EFS data collection script should be used for EFS encryptio/decryption problems. The script will collect EFS releavnt ETL traces, procmon logs and psr recording of the problem repro steps. Tracing time should be minimzied, otherwise procmon logs will get very large. In additoin to EFS data collection scripts please collect Authentication data collection script. In addition to that get the "cipher /c path_of_the_file_in_repro"</t>
@@ -185,6 +164,27 @@
 - TSS ensures consistent data sets with timestamps in log file and PSR
 - automatic stop trigger when investigating intermittent issues (no repro at will)
 The More Information section is included in the current version of the word doc contained in tss_tools_v1.*.zip and tss_tools_ttt_v1.*.zip</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Milan</t>
+  </si>
+  <si>
+    <t>Tolu</t>
+  </si>
+  <si>
+    <t>Bousso; Tolu</t>
+  </si>
+  <si>
+    <t>Marius</t>
+  </si>
+  <si>
+    <t>Marius; Milan</t>
+  </si>
+  <si>
+    <t>Wayne</t>
   </si>
 </sst>
 </file>
@@ -581,20 +581,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.88671875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,173 +623,173 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
       <c r="I3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
       <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
+    </row>
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="11" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="6" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -802,19 +802,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9EADDC-B7C3-4DA1-ABDD-21E6149184D4}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,28 +828,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -866,9 +866,9 @@
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,30 +882,30 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -922,9 +922,9 @@
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -938,30 +938,30 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -978,9 +978,9 @@
       <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -994,30 +994,30 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1034,9 +1034,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1050,30 +1050,30 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dummy internal package added
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ADS" sheetId="1" r:id="rId1"/>
@@ -220,9 +220,6 @@
     <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/NET/TSS/TSS.zip?raw=true</t>
   </si>
   <si>
-    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/PRF/Package1/Package1.zip?raw=true</t>
-  </si>
-  <si>
     <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/PRF/Package2/Package2.zip?raw=true</t>
   </si>
   <si>
@@ -310,6 +307,9 @@
   </si>
   <si>
     <t xml:space="preserve">The purpose of this tool is following...when you collect several event logs from a server and you don't know yet what to look for, and can be tedious to load all of </t>
+  </si>
+  <si>
+    <t>\\dummymachine\dummyinternalshare\Package1.zip</t>
   </si>
 </sst>
 </file>
@@ -728,7 +728,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,7 +758,7 @@
         <v>47</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -791,7 +791,7 @@
         <v>48</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G2">
         <v>9</v>
@@ -823,7 +823,7 @@
         <v>49</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -855,7 +855,7 @@
         <v>50</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -890,7 +890,7 @@
         <v>51</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -913,7 +913,7 @@
         <v>52</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -934,7 +934,7 @@
         <v>53</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -957,7 +957,7 @@
         <v>54</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -975,7 +975,7 @@
         <v>55</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -996,7 +996,7 @@
         <v>56</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1042,7 +1042,7 @@
         <v>47</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
@@ -1060,43 +1060,43 @@
         <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="300" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1142,43 +1142,43 @@
         <v>47</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1195,13 +1195,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="41.140625" customWidth="1"/>
+    <col min="5" max="5" width="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
         <v>47</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1236,10 +1236,10 @@
         <v>32</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1256,10 +1256,10 @@
         <v>31</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1302,7 +1302,7 @@
         <v>47</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1317,10 +1317,10 @@
         <v>32</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1337,10 +1337,10 @@
         <v>31</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1383,7 +1383,7 @@
         <v>47</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1398,10 +1398,10 @@
         <v>32</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1418,10 +1418,10 @@
         <v>31</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1438,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,10 +1466,10 @@
         <v>47</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="405" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
@@ -1484,61 +1484,61 @@
         <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="300" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating crutil and xlsx
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99AC93C-08CA-4347-95F5-1F5F75A3E583}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5976AE-DE5A-4453-B322-48CFCB1EA5A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="1305" windowWidth="21600" windowHeight="14640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1455" yWindow="1380" windowWidth="27120" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADS" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -336,6 +336,21 @@
   </si>
   <si>
     <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/SHA/Hyper-V_Tracing_Using_Channels/Hyper-V_Tracing_Using_Channels.zip?raw=true</t>
+  </si>
+  <si>
+    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/ADS/PKI_Credential_Roaming_Util/CRUtil.zip?raw=true</t>
+  </si>
+  <si>
+    <t>Credential Roaming Utility (crutil) is tool for extracting the credential roaming relevant data from the AD user account, troubleshooting credential roaming issues and AD database size root cause analysis.
+The tool must be executed in the security context of the account that has read rights for AD user account of the user whose credential roaming AD data needs to be investigated. After specifying username and domainname (and optionally domain controller) and clicking "Get Credential Roaming AD User Data" button in the UI, the tool will generate CredRoamLogs folder (in the same folder where app binary is placed) and collect four csv files:
+UserCredRoamADObjData.csv with user's AD object relevant info: User_Name, User_Email_Addresses, User_Distinguisehd_Name, MsPKITimeCreationDate, MsPKITimeModifiedDate and PwdLastSetDateTime
+UserCredRoamADAttrData.csv with user's AD credential roaming attributes relevant info (please note that this information is stored as BLOB in AD): DIMS_Roaming_Status, Token_Type, Token_ID, Token_Size, Last_Roamed, Key_Info, Cert_Subject, Cert_Issuer and Cert_Template (Cert_Subject, Cert_Issuer, Cert_Template will be set to "not applicable" if the inspected BLOB value is not certificate)
+UserCredRoamLVRAttrData.csv with user's AD object relevant info: User_Name, User_Email_Addresses, User_Distinguisehd_Name, Version, Time_LastOrigChange, USN_Local_Change, USN_Originating_Change
+UserCredRoamLVRObjData.csv with user's AD credential roaming attributes relevant infos (please note that this information is stored as BLOB in AD): DIMS_Roaming_Status, Token_Type, Token_ID, Token_Size, Last_Roamed, Key_Info, Cert_Subject, Cert_Issuer, Cert_Template (Cert_Subject, Cert_Issuer, Cert_Template will be set to "not applicable" if the inspected BLOB value is not certificate)
+For more information about credential roaming technology, please refer to: https://social.technet.microsoft.com/wiki/contents/articles/11483.windows-credential-roaming.aspx https://blogs.technet.microsoft.com/askds/2009/01/06/certs-on-wheels-understanding-credential-roaming/</t>
+  </si>
+  <si>
+    <t>PKI_Credential_Roaming_Util</t>
   </si>
 </sst>
 </file>
@@ -751,23 +766,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.88671875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="6" width="64.6640625" customWidth="1"/>
-    <col min="7" max="11" width="25.5546875" customWidth="1"/>
+    <col min="1" max="1" width="59.28515625" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="6" width="64.7109375" customWidth="1"/>
+    <col min="7" max="11" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>35</v>
       </c>
@@ -832,7 +847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
@@ -864,7 +879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
@@ -899,7 +914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -922,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -945,7 +960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>20</v>
       </c>
@@ -966,71 +981,90 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="6" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{7C9D4DF6-0513-4A75-B449-1C2C8F2F8709}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1042,16 +1076,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1105,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
@@ -1089,7 +1123,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>70</v>
       </c>
@@ -1107,7 +1141,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="300" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>73</v>
       </c>
@@ -1140,18 +1174,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="42.44140625" customWidth="1"/>
-    <col min="5" max="5" width="68.88671875" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +1205,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>64</v>
       </c>
@@ -1189,7 +1223,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>65</v>
       </c>
@@ -1207,7 +1241,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="360" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="405" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>81</v>
       </c>
@@ -1244,12 +1278,12 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1269,7 +1303,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
@@ -1287,7 +1321,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
@@ -1325,12 +1359,12 @@
       <selection activeCell="F1" sqref="F1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1350,7 +1384,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
@@ -1368,7 +1402,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
@@ -1406,12 +1440,12 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1431,7 +1465,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
@@ -1449,7 +1483,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
@@ -1487,14 +1521,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="65.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1514,7 +1548,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="405" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
@@ -1532,7 +1566,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>64</v>
       </c>
@@ -1550,7 +1584,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>65</v>
       </c>
@@ -1568,7 +1602,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="300" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Update of Links in ALL, NET
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20343"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261B00F8-928C-4258-9069-28D3B6C1DFF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400F3A00-C2B4-4238-9C78-911C43AB9829}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43170" windowHeight="19005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ADS" sheetId="1" r:id="rId1"/>
-    <sheet name="NET" sheetId="2" r:id="rId2"/>
-    <sheet name="SHA" sheetId="3" r:id="rId3"/>
-    <sheet name="PRF" sheetId="4" r:id="rId4"/>
-    <sheet name="UEX" sheetId="5" r:id="rId5"/>
-    <sheet name="DND" sheetId="6" r:id="rId6"/>
-    <sheet name="ALL" sheetId="7" r:id="rId7"/>
+    <sheet name="ALL" sheetId="7" r:id="rId1"/>
+    <sheet name="ADS" sheetId="1" r:id="rId2"/>
+    <sheet name="NET" sheetId="2" r:id="rId3"/>
+    <sheet name="SHA" sheetId="3" r:id="rId4"/>
+    <sheet name="PRF" sheetId="4" r:id="rId5"/>
+    <sheet name="UEX" sheetId="5" r:id="rId6"/>
+    <sheet name="DND" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -147,21 +147,6 @@
   </si>
   <si>
     <t>TSS</t>
-  </si>
-  <si>
-    <t>TSS TroubleShootingScript/toolset for rapid flexible data collection for CritSit and standard cases. This TSS TroubleShootingScript/toolset aims for rapid data collection for CritSit and standard cases.
-Download share: \\emeaCssDfs\netpod\Tools-Scripts\Troubleshooting-Script\ - please always downlaod latest available tss_tools_v1.*.zip
-Because of the bigger size, there is a separate zip, which includes iDNA/TTT binaries: in sub folder \TTT\tss_tools_ttt_v1.*.zip, which includes TTT_x86_x64_external.zip
-TSS Goal: helping you to collect data and solve incidents in the shortest timeframe
-Internal + external tss_tools_v*.zip-integrated documentation: tss.cmd_ReadMe_Help.docx
-Benefits of using TSS for many cases/customer incidents
-- for all involved parties: huge time saver working on SRs
-- for customer, no complicated manual action plans
-- for engineer, no need for writing long action plans, discussing plan on phone
-- for Backline SEE/EE no lengthy handover discussion on available/or missing data
-- TSS ensures consistent data sets with timestamps in log file and PSR
-- automatic stop trigger when investigating intermittent issues (no repro at will)
-The More Information section is included in the current version of the word doc contained in tss_tools_v1.*.zip and tss_tools_ttt_v1.*.zip</t>
   </si>
   <si>
     <t>Nick</t>
@@ -302,9 +287,6 @@
   </si>
   <si>
     <t>\\dummymachine\dummyinternalshare\Package1.zip</t>
-  </si>
-  <si>
-    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/NET/TSS/tss_tools_v1.80.06.zip?raw=true</t>
   </si>
   <si>
     <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/ALL/psSDP/psSDP-offline.zip?raw=true</t>
@@ -374,6 +356,58 @@
   </si>
   <si>
     <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/ADS/PKI_CRUtil/CRUtil.zip?raw=true</t>
+  </si>
+  <si>
+    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/ALL/TSS/tss_tools.zip?raw=true</t>
+  </si>
+  <si>
+    <t>TSS TroubleShootingScript/toolset for rapid flexible data collection for CritSit and standard cases. This TSS TroubleShootingScript/toolset aims for rapid data collection for CritSit and standard cases.  - Please always downlaod latest availabe package
+Because of the bigger size, there is a separate zip, which includes iDNA/TTT binaries: in sub folder \TTT\tss_tools_ttt.zip, which includes TTT_x86_x64_external.zip
+TSS Goal: helping you to collect data and solve incidents in the shortest timeframe
+Internal + external tss_tools.zip-integrated documentation: tss.cmd_ReadMe_Help.docx
+Benefits of using TSS for many cases/customer incidents
+- for all involved parties: huge time saver working on SRs
+- for customer, no complicated manual action plans
+- for engineer, no need for writing long action plans, discussing plan on phone
+- for Backline SEE/EE no lengthy handover discussion on available/or missing data
+- TSS ensures consistent data sets with timestamps in log file and PSR
+- automatic stop trigger when investigating intermittent issues (no repro at will)
+The More Information section is included in the current version of the word doc contained in tss_tools.zip and tss_tools_ttt.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psSDP is PowerShell based SDP (Support Diagnostic Package) as an alternative to traditional Microsoft **Support Diagnostic Packages**
+Purpose
+Collect **SDP** speciality report on Microsoft Windows systems
+Usage
+To start data collection, run in an elevated PowerShell window
+ ` .\get-psSDP.ps1 [Net|Dom|CTS|Print|HyperV|Setup|Cluster|Perf|SQLbase|Mini|Nano] `
+ Example for SDP Networking Diagnostic:  
+  `.\get-psSDP.ps1 Net`
+ Example for SDP Basic (mini) data collection: 
+ `.\get-psSDP.ps1 Mini`
+  Example for SDP Net without zipping results:
+  `.\get-psSDP.ps1 Net NoCab`
+</t>
+  </si>
+  <si>
+    <t>TSS_tools_ttt</t>
+  </si>
+  <si>
+    <t>TSS TroubleShootingScript/toolset for rapid flexible data collection for CritSit and standard cases. This TSS TroubleShootingScript/toolset aims for rapid data collection for CritSit and standard cases.  - Please always downlaod latest availabe package
+Because of the bigger size, this is a separate zip, which includes iDNA/TTT binaries: in sub folder \TTD\tss_tools_ttt.zip, which includes TTT_x86_x64_external.zip
+TSS Goal: helping you to collect data and solve incidents in the shortest timeframe
+Internal + external tss_tools_ttt.zip-integrated documentation: tss.cmd_ReadMe_Help.docx
+Benefits of using TSS for many cases/customer incidents
+- for all involved parties: huge time saver working on SRs
+- for customer, no complicated manual action plans
+- for engineer, no need for writing long action plans, discussing plan on phone
+- for Backline SEE/EE no lengthy handover discussion on available/or missing data
+- TSS ensures consistent data sets with timestamps in log file and PSR
+- automatic stop trigger when investigating intermittent issues (no repro at will)
+The More Information section is included in the current version of the word doc contained in tss_tools_ttt.zip</t>
+  </si>
+  <si>
+    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/ALL/TSS/TTD/tss_tools_ttt.zip?raw=true</t>
   </si>
 </sst>
 </file>
@@ -510,8 +544,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -788,14 +822,153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="390" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="390" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{71692038-50AB-4468-B343-A9A55863E0E3}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{5CD8526D-0FAD-4C89-8AC2-6C315B7E87A3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.28515625" customWidth="1"/>
     <col min="2" max="2" width="91.28515625" style="5" customWidth="1"/>
@@ -819,10 +992,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -849,13 +1022,13 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2">
         <v>9</v>
@@ -881,13 +1054,13 @@
         <v>35</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -913,13 +1086,13 @@
         <v>35</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -942,19 +1115,19 @@
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -971,13 +1144,13 @@
         <v>35</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -992,13 +1165,13 @@
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -1006,38 +1179,38 @@
     </row>
     <row r="8" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1051,13 +1224,13 @@
         <v>35</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1072,13 +1245,13 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1090,13 +1263,13 @@
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1110,15 +1283,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64.5703125" customWidth="1"/>
@@ -1141,64 +1314,64 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="390" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="300" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1212,15 +1385,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="42.42578125" customWidth="1"/>
@@ -1241,64 +1414,64 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>68</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="405" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1312,7 +1485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1320,7 +1493,7 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="58" customWidth="1"/>
   </cols>
@@ -1339,10 +1512,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1357,10 +1530,10 @@
         <v>31</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1377,10 +1550,10 @@
         <v>30</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1393,7 +1566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1401,7 +1574,7 @@
       <selection activeCell="F1" sqref="F1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
@@ -1420,10 +1593,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1438,10 +1611,10 @@
         <v>31</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1458,10 +1631,10 @@
         <v>30</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1474,7 +1647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1482,7 +1655,7 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
   </cols>
@@ -1501,10 +1674,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1519,10 +1692,10 @@
         <v>31</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1539,10 +1712,10 @@
         <v>30</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1553,123 +1726,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="405" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="300" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Uploaded ClusterHiveReaderFromClusterLog.ps1; Updated GetLogs.ps1; updated Windows_PODs.xls
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5859392-6DCD-4D5F-8DA6-89D715CDBF9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5352FD-FABC-4D82-82E3-8DF3D4612CEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="810" windowWidth="27285" windowHeight="15915" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28245" yWindow="945" windowWidth="28065" windowHeight="15765" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -668,6 +668,38 @@
   </si>
   <si>
     <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/SHA/StorPortPacman/StorPortPacman.zip?raw=true</t>
+  </si>
+  <si>
+    <t>ClusterHiveReaderFromClusterLog.ps1</t>
+  </si>
+  <si>
+    <t>Purpose: 
+# SYNOPSIS ClusterHiveReaderFromClusterLog.ps1
+    The script Reads the Header Lines from a Server 2016 or later cluster.log and creates config files
+    Script Name:  ClusterHiveReaderFromClusterLog.ps1    	
+    Version:      1.1
+    Last Update:  12 Feb 2020
+    Author:       Josef Holzer 
+## DESCRIPTION
+    In 2016 and later we store all Configuration Info on top of the Cluster Log in csv format
+    The script reads the header of the cluster.log file and creates the following files:    
+    ClusterLogName-ClusConfig-All.txt             # Contains all Info Exported as AllObjects  fl *
+    ClusterLogName-ClusConfig-All.xml             # Contains all Info as Powershell Objects
+    ClusterLogName-ClusConfig-All-Overview.txt    # Contains most important info as | ft Prop1, Prop2...
+    ClusterLogName-ClusConfig-ProcessIDs.txt      # All PIDs of Processes that wrote to cluster log
+EXAMPLE 1
+     ClusterHiveReaderFromClusterLog.ps1    
+    - if you have several cluster logs in c:\logs and copy the script to this folder
+       you simply run the script with no parameters
+    - it will then take the first (2016 or later ) 
+      cluster.log that contains config data and processes it
+EXAMPLE 2
+    ClusterHiveReaderFromClusterLog.ps1 -Path "C:\ClusterLog\H19N1.H19Corp.com_cluster.log" `
+    -FileWithProcessInfoPathFull "C:\ClusterLog\H19N1-GeneralInfoPerHost.xml" -FindPIDs $True
+    ...it will read cluster configuration and write it down into file names mentioned above including *ProcessIDs</t>
+  </si>
+  <si>
+    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/SHA/ClusterHiveReaderFromClusterLog/ClusterHiveReaderFromClusterLog.zip?raw=true</t>
   </si>
 </sst>
 </file>
@@ -1875,10 +1907,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1997,15 +2029,32 @@
         <v>86</v>
       </c>
     </row>
+    <row r="7" spans="1:6" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{A409CFB4-8861-4EDF-83F2-7EC982978C7C}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{9F94F2E5-8767-4F52-9EEF-AC692ECF310F}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{88B198AD-A8B9-4F55-9F69-56BB5E1EE4C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added DNS_SUFFIX_RESET.EXE Tool To ALL/MISC
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B068E9B-2618-44DD-B624-31D2CB514354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3D4C0D-1736-46B0-A461-FFEF1648DCFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="24585" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="180">
   <si>
     <t>Name</t>
   </si>
@@ -743,6 +743,25 @@
   </si>
   <si>
     <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/PRF/Perfomance_Counters/Perf-Collect.zip?raw=true</t>
+  </si>
+  <si>
+    <t>DNS_SUFFIX_RESET</t>
+  </si>
+  <si>
+    <t>When connected to MSFTVPN, I cannot access internal resources like HRWeb, RAMWeb, or others. What should I do?
+​​	To be able to reach internal resources like those mentioned above, follow the steps below.
+	- To resolve this issue, you'll need to run a script on the device. To get started, double-click on DNS_SUFFIX_RESET.EXE. 
+	- You will be prompted to run the script. Select Run.
+	- You will be asked for confirmation to proceed. Select Yes.
+	- The script will then run to completion. Once the script is complete, press any key to close the window.
+	- If you are still unable to access internal resources, please contact the Helpdesk and inform them that you have followed the steps above. 
+	  Ask them to escalate this issue. Please DO NOT complete the steps above f​or a second time.</t>
+  </si>
+  <si>
+    <t>StefanG</t>
+  </si>
+  <si>
+    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/ALL/MISC/DNS_SUFFIX_RESET.zip?raw=true</t>
   </si>
 </sst>
 </file>
@@ -882,8 +901,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1161,15 +1180,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
     <col min="5" max="5" width="34.85546875" customWidth="1"/>
     <col min="6" max="6" width="30.5703125" customWidth="1"/>
@@ -1354,6 +1373,24 @@
         <v>134</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1382,7 +1419,7 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.28515625" customWidth="1"/>
     <col min="2" max="2" width="91.28515625" style="5" customWidth="1"/>
@@ -1798,7 +1835,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64.5703125" customWidth="1"/>
@@ -1956,7 +1993,7 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="119.28515625" customWidth="1"/>
@@ -2105,11 +2142,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="58" customWidth="1"/>
   </cols>
@@ -2169,7 +2206,7 @@
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
@@ -2365,7 +2402,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="65.140625" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
removed old nm parserd and updates d xlsx
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3D4C0D-1736-46B0-A461-FFEF1648DCFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2E69CE-ADEF-44F0-9CD6-FD8557180D45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="24585" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="7" r:id="rId1"/>
@@ -342,9 +342,6 @@
   </si>
   <si>
     <t>Analysis and Troubleshooting</t>
-  </si>
-  <si>
-    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/NET/NetworkMonitor_Parsers_03_04_2978_x64/NetworkMonitor_Parsers_03_04_2978_x64.zip?raw=true</t>
   </si>
   <si>
     <t>NetMon Parser</t>
@@ -762,6 +759,9 @@
   </si>
   <si>
     <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/ALL/MISC/DNS_SUFFIX_RESET.zip?raw=true</t>
+  </si>
+  <si>
+    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/NET/NetworkMonitor_Parsers_Internal_03_04_2990/NetworkMonitor_Parsers_Internal_03_04_2990.zip?raw=true</t>
   </si>
 </sst>
 </file>
@@ -901,8 +901,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1182,11 +1182,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
@@ -1219,7 +1219,7 @@
         <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
@@ -1237,7 +1237,7 @@
         <v>79</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
@@ -1306,17 +1306,17 @@
     </row>
     <row r="7" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>52</v>
@@ -1324,35 +1324,35 @@
     </row>
     <row r="8" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>52</v>
@@ -1360,38 +1360,38 @@
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1419,7 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.28515625" customWidth="1"/>
     <col min="2" max="2" width="91.28515625" style="5" customWidth="1"/>
@@ -1505,7 +1505,7 @@
         <v>32</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>42</v>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>45</v>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>46</v>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>75</v>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>71</v>
@@ -1705,17 +1705,17 @@
     </row>
     <row r="12" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>53</v>
@@ -1723,17 +1723,17 @@
     </row>
     <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>53</v>
@@ -1741,17 +1741,17 @@
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>52</v>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>49</v>
@@ -1777,17 +1777,17 @@
     </row>
     <row r="16" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>52</v>
@@ -1795,17 +1795,17 @@
     </row>
     <row r="17" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>52</v>
@@ -1831,11 +1831,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64.5703125" customWidth="1"/>
@@ -1920,17 +1920,17 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>116</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>52</v>
@@ -1938,17 +1938,17 @@
     </row>
     <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>52</v>
@@ -1956,17 +1956,17 @@
     </row>
     <row r="7" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>52</v>
@@ -1993,7 +1993,7 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="119.28515625" customWidth="1"/>
@@ -2061,17 +2061,17 @@
     </row>
     <row r="4" spans="1:6" ht="327" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>148</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>149</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>52</v>
@@ -2079,15 +2079,15 @@
     </row>
     <row r="5" spans="1:6" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>52</v>
@@ -2095,15 +2095,15 @@
     </row>
     <row r="6" spans="1:6" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>81</v>
@@ -2111,15 +2111,15 @@
     </row>
     <row r="7" spans="1:6" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>81</v>
@@ -2146,7 +2146,7 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="58" customWidth="1"/>
   </cols>
@@ -2173,17 +2173,17 @@
     </row>
     <row r="2" spans="1:6" ht="255" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>52</v>
@@ -2206,7 +2206,7 @@
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
@@ -2236,17 +2236,17 @@
     </row>
     <row r="2" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>52</v>
@@ -2254,17 +2254,17 @@
     </row>
     <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>125</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>52</v>
@@ -2272,17 +2272,17 @@
     </row>
     <row r="4" spans="1:6" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>52</v>
@@ -2290,17 +2290,17 @@
     </row>
     <row r="5" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>52</v>
@@ -2308,17 +2308,17 @@
     </row>
     <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>52</v>
@@ -2326,17 +2326,17 @@
     </row>
     <row r="7" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>165</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>52</v>
@@ -2344,17 +2344,17 @@
     </row>
     <row r="8" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>52</v>
@@ -2362,17 +2362,17 @@
     </row>
     <row r="9" spans="1:6" ht="270" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>52</v>
@@ -2402,7 +2402,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="65.140625" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
@@ -2430,17 +2430,17 @@
     </row>
     <row r="2" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>128</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>129</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
removed setupreport from ads
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2896EC8E-F95B-4DF8-8A62-215A8164C844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D706427-D50F-4969-B4A9-E859561D37F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4365" yWindow="2055" windowWidth="21600" windowHeight="11535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="185">
   <si>
     <t>Name</t>
   </si>
@@ -787,12 +787,6 @@
 ## DESCRIPTION
 shacollector is a tool that makes it easy to collect data for problem solving which is included in trace logs (ETW), 
 performance logs (perfmon or xperf), event logs and a lot of status information related to SHA area (Storage, Cluster and Hyper-V).</t>
-  </si>
-  <si>
-    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/ADS/SetupReport/SetupReport.zip?raw=true</t>
-  </si>
-  <si>
-    <t>SetupReprot description</t>
   </si>
 </sst>
 </file>
@@ -1444,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,24 +1836,6 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -1871,10 +1847,9 @@
     <hyperlink ref="E16" r:id="rId7" xr:uid="{3B3A1A78-FE12-44AD-BC50-B9F31B170A4D}"/>
     <hyperlink ref="E17" r:id="rId8" xr:uid="{4E649777-4D45-4326-A92A-E9A481BFE847}"/>
     <hyperlink ref="E2" r:id="rId9" xr:uid="{2456CD6B-AEAB-4A1D-A2CF-C48240CAE1BC}"/>
-    <hyperlink ref="E18" r:id="rId10" xr:uid="{74D5C6DD-4AB9-4EBC-99FD-771C562A0C23}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding UXtrace to the inventory file
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D706427-D50F-4969-B4A9-E859561D37F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4287BC3-6C02-4EC6-9973-1EB9D121436D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="2055" windowWidth="21600" windowHeight="11535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="189">
   <si>
     <t>Name</t>
   </si>
@@ -787,6 +787,19 @@
 ## DESCRIPTION
 shacollector is a tool that makes it easy to collect data for problem solving which is included in trace logs (ETW), 
 performance logs (perfmon or xperf), event logs and a lot of status information related to SHA area (Storage, Cluster and Hyper-V).</t>
+  </si>
+  <si>
+    <t>UXTrace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryutaro Hayashi </t>
+  </si>
+  <si>
+    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/UXTrace/UXTrace.ps1?raw=true
+https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WinRM/WinRM-Diag.zip?raw=true</t>
+  </si>
+  <si>
+    <t>UXTrace is a uniformed tool to collect traces and logs in customer environment. You can collect all diagnostic traces below at the same time and flexibly. It allows to capture "Logman" traces (mostly for main UEX components) , WPR, Procmon, Netsh,TTD,Recorder</t>
   </si>
 </sst>
 </file>
@@ -889,7 +902,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -924,10 +937,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1211,7 +1230,7 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
@@ -1440,11 +1459,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.28515625" customWidth="1"/>
     <col min="2" max="2" width="91.28515625" style="5" customWidth="1"/>
@@ -1861,7 +1880,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64.5703125" customWidth="1"/>
@@ -2019,7 +2038,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="119.28515625" customWidth="1"/>
@@ -2193,7 +2212,7 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="58" customWidth="1"/>
   </cols>
@@ -2247,13 +2266,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
@@ -2425,6 +2444,24 @@
         <v>51</v>
       </c>
     </row>
+    <row r="10" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
@@ -2435,9 +2472,10 @@
     <hyperlink ref="E7" r:id="rId6" xr:uid="{9A1DB91A-6547-4DA8-8EC0-B699AB3318C0}"/>
     <hyperlink ref="E8" r:id="rId7" display="https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WMI-Collect/WMI-Collect.zip?raw=true" xr:uid="{25497EC0-956A-4C27-8920-6C36A5988903}"/>
     <hyperlink ref="E9" r:id="rId8" display="https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WMI-Collect/WMI-Collect.zip?raw=true" xr:uid="{E30A40E0-D4AE-4049-BEBB-A967B83D0710}"/>
+    <hyperlink ref="E10" r:id="rId9" display="https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WMI-Collect/WMI-Collect.zip?raw=true" xr:uid="{412BCE25-98C7-4B25-94EB-1AC9331687AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -2449,7 +2487,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="65.140625" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Adding UXTrace to the inventory
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4287BC3-6C02-4EC6-9973-1EB9D121436D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CA4909-8F0A-4813-AC58-3F7A227268C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -799,7 +799,7 @@
 https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WinRM/WinRM-Diag.zip?raw=true</t>
   </si>
   <si>
-    <t>UXTrace is a uniformed tool to collect traces and logs in customer environment. You can collect all diagnostic traces below at the same time and flexibly. It allows to capture "Logman" traces (mostly for main UEX components) , WPR, Procmon, Netsh,TTD,Recorder</t>
+    <t>UXTrace is a powershell script to capture traces and collect data for troubleshooting. You can capture traces for UEX components like shell(explorer) and AppX. Also OS basic information and component data/settings can collect with this script.  WPR, ProcMon,IDNA traces can be captured as well.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added the Printing tools
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B706E1B5-2864-4F0B-8EBC-19209C78F5D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED15AA91-DC7C-47BE-8683-EC9326B5AADB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="196">
   <si>
     <t>Name</t>
   </si>
@@ -808,6 +808,20 @@
   </si>
   <si>
     <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/ADS/ADS_DatabaseAnalyzer_public/ADS_DatabaseAnalyzer_public.zip?raw=true</t>
+  </si>
+  <si>
+    <t>Printing</t>
+  </si>
+  <si>
+    <t>Contains printing tools. Print-Collect will gather data to investigate a printing issue. Print-CollectA is a lighter version. Print-Trace will collect traces (ETL,Procmon,PSR, network trace). Print-Trace-local.bat will not capture network traces.</t>
+  </si>
+  <si>
+    <t>luct</t>
+  </si>
+  <si>
+    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/Printing/Print-Collect.zip?raw=true
+https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/Printing/Print-CollectA.zip?raw=true
+https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/Printing/Print-Trace.zip?raw=true</t>
   </si>
 </sst>
 </file>
@@ -910,7 +924,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -951,10 +965,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1238,7 +1253,7 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
@@ -1467,11 +1482,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+    <sheetView topLeftCell="C22" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.28515625" customWidth="1"/>
     <col min="2" max="2" width="91.28515625" style="5" customWidth="1"/>
@@ -1907,7 +1922,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64.5703125" customWidth="1"/>
@@ -2065,7 +2080,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="119.28515625" customWidth="1"/>
@@ -2239,7 +2254,7 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="58" customWidth="1"/>
   </cols>
@@ -2293,13 +2308,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
@@ -2435,7 +2450,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>165</v>
       </c>
@@ -2488,6 +2503,26 @@
       <c r="F10" s="15" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2500,9 +2535,10 @@
     <hyperlink ref="E8" r:id="rId7" display="https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WMI-Collect/WMI-Collect.zip?raw=true" xr:uid="{25497EC0-956A-4C27-8920-6C36A5988903}"/>
     <hyperlink ref="E9" r:id="rId8" display="https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WMI-Collect/WMI-Collect.zip?raw=true" xr:uid="{E30A40E0-D4AE-4049-BEBB-A967B83D0710}"/>
     <hyperlink ref="E10" r:id="rId9" xr:uid="{412BCE25-98C7-4B25-94EB-1AC9331687AF}"/>
+    <hyperlink ref="E11" r:id="rId10" display="https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WMI-Collect/WMI-Collect.zip?raw=true" xr:uid="{A271FA40-3139-4A12-A942-63D5CDA85A29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -2514,7 +2550,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="65.140625" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Updated to correct UEX issues
</commit_message>
<xml_diff>
--- a/Windows_PODs.xlsx
+++ b/Windows_PODs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCDE176-B34C-4406-960C-8D9168F12AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FD7616-725A-4003-ADF3-9B316972D256}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16275" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12525" yWindow="-16350" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="196">
   <si>
     <t>Name</t>
   </si>
@@ -715,19 +715,11 @@
 WMI-Collect: PowerShell script that collects WMI relevant data</t>
   </si>
   <si>
-    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WMI/WMI-Report.zip?raw=true
-https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WMI/WMI-Collect.zip?raw=true</t>
-  </si>
-  <si>
     <t>WinRM</t>
   </si>
   <si>
     <t>WinRM-Collect: PowerShell script to simplify the collection of WinRM and EventLog Forwarding troubleshooting data and make our action plans easier.
 WinRM-Diag: PowerShell script that inspects the WinRM configuration and tries to identify common issues.</t>
-  </si>
-  <si>
-    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WinRM/WinRM-Collect.zip?raw=true
-https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WinRM/WinRM-Diag.zip?raw=true</t>
   </si>
   <si>
     <t>Perf-Collect</t>
@@ -808,6 +800,25 @@
   </si>
   <si>
     <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/ADS/ADS_DatabaseAnalyzer_public/ADS_DatabaseAnalyzer_public.zip?raw=true</t>
+  </si>
+  <si>
+    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WMI/WMI.zip?raw=true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WinRM/WinRM.zip?raw=true
+</t>
+  </si>
+  <si>
+    <t>Printing</t>
+  </si>
+  <si>
+    <t>Contains printing tools. Print-Collect will gather data to investigate a printing issue. Print-CollectA is a lighter version. Print-Trace will collect traces (ETL,Procmon,PSR, network trace). Print-Trace-local.bat will not capture network traces.</t>
+  </si>
+  <si>
+    <t>luct</t>
+  </si>
+  <si>
+    <t>https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/Printing/Print.zip?raw=true</t>
   </si>
 </sst>
 </file>
@@ -910,7 +921,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -948,10 +959,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1431,17 +1441,17 @@
     </row>
     <row r="11" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>131</v>
@@ -1468,7 +1478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="C22" workbookViewId="0">
+    <sheetView topLeftCell="C13" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1529,7 +1539,7 @@
         <v>35</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>51</v>
@@ -1866,17 +1876,17 @@
     </row>
     <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="6" t="s">
         <v>96</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>52</v>
@@ -2021,7 +2031,7 @@
         <v>83</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>51</v>
@@ -2062,7 +2072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2191,7 +2201,7 @@
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>155</v>
@@ -2202,17 +2212,17 @@
     </row>
     <row r="8" spans="1:6" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>80</v>
@@ -2267,17 +2277,17 @@
     </row>
     <row r="2" spans="1:6" ht="255" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
         <v>117</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>51</v>
@@ -2294,17 +2304,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
-    <col min="5" max="5" width="69" customWidth="1"/>
+    <col min="5" max="5" width="95.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2418,7 +2428,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>162</v>
       </c>
@@ -2436,7 +2446,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>165</v>
       </c>
@@ -2448,50 +2458,71 @@
         <v>117</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="270" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
         <v>117</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>187</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E11" s="16"/>
+      <c r="F10" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2501,12 +2532,13 @@
     <hyperlink ref="E5" r:id="rId4" xr:uid="{C4372465-92F8-4B6D-B622-F870635B66EF}"/>
     <hyperlink ref="E6" r:id="rId5" xr:uid="{F8D3BCE4-9CF0-450A-9D11-402B8A0468F5}"/>
     <hyperlink ref="E7" r:id="rId6" xr:uid="{9A1DB91A-6547-4DA8-8EC0-B699AB3318C0}"/>
-    <hyperlink ref="E8" r:id="rId7" display="https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WMI-Collect/WMI-Collect.zip?raw=true" xr:uid="{25497EC0-956A-4C27-8920-6C36A5988903}"/>
-    <hyperlink ref="E9" r:id="rId8" display="https://github.com/CSS-Windows/WindowsDiag/blob/master/UEX/WMI-Collect/WMI-Collect.zip?raw=true" xr:uid="{E30A40E0-D4AE-4049-BEBB-A967B83D0710}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{25497EC0-956A-4C27-8920-6C36A5988903}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{E30A40E0-D4AE-4049-BEBB-A967B83D0710}"/>
     <hyperlink ref="E10" r:id="rId9" xr:uid="{412BCE25-98C7-4B25-94EB-1AC9331687AF}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{29ADC959-5972-420A-98DA-87D8B98AD639}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>